<commit_message>
add accounting format example
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/numberFormat.xlsx
+++ b/src/main/webapp/WEB-INF/books/numberFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/DOC/zssessentials/src/main/webapp/WEB-INF/books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B0DCED-A54F-F54D-8003-E7B369E4862C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395094AF-7D51-B941-8F52-1ED57AFB3E34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="az_ReportName">Sheet1!$A$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>dd/mm/yyyy hh:mm</t>
   </si>
@@ -88,13 +88,17 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Accounting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mmm\-dd"/>
@@ -102,6 +106,7 @@
     <numFmt numFmtId="168" formatCode="dd/mm/yyyy\,\ dddd"/>
     <numFmt numFmtId="169" formatCode="dd/mm/yyyy\ hh:mm;@"/>
     <numFmt numFmtId="170" formatCode="[$$-409]#,##0.00"/>
+    <numFmt numFmtId="171" formatCode="_ [$₹-439]\ * #,##0.00_ ;_ [$₹-439]\ * \-#,##0.00_ ;_ [$₹-439]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -172,7 +177,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -200,6 +205,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -516,16 +524,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="17" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="30.1640625" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -653,6 +661,19 @@
         <v>123456789</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="18">
+        <v>123.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>